<commit_message>
Headings that make some sort of sense
</commit_message>
<xml_diff>
--- a/Engineering/ARAP/Flying_ARAP.xlsx
+++ b/Engineering/ARAP/Flying_ARAP.xlsx
@@ -27,17 +27,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>bits per second</t>
+    <t>2m symbol rate</t>
+  </si>
+  <si>
+    <t>How much?</t>
+  </si>
+  <si>
+    <t>Units?</t>
+  </si>
+  <si>
+    <t>What is it?</t>
+  </si>
+  <si>
+    <t>bps</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -65,8 +85,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -344,23 +370,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
         <v>9600</v>
       </c>
-      <c r="C2" t="s">
-        <v>0</v>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added "how many bits left over" column to see if there are any.
There aren’t for several rates.
</commit_message>
<xml_diff>
--- a/Engineering/ARAP/Flying_ARAP.xlsx
+++ b/Engineering/ARAP/Flying_ARAP.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17340" yWindow="8220" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="18940" yWindow="7140" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>2m symbol rate</t>
   </si>
@@ -42,6 +42,60 @@
   </si>
   <si>
     <t>bps</t>
+  </si>
+  <si>
+    <t>CODEC2 3200 bps</t>
+  </si>
+  <si>
+    <t>CODEC2 2400 bps</t>
+  </si>
+  <si>
+    <t>CODEC2 1600 bps</t>
+  </si>
+  <si>
+    <t>CODEC2 1400 bps</t>
+  </si>
+  <si>
+    <t>CODEC2 1300 bps</t>
+  </si>
+  <si>
+    <t>CODEC2 1200 bps</t>
+  </si>
+  <si>
+    <t>CODEC2 700 bps</t>
+  </si>
+  <si>
+    <t>Channels?</t>
+  </si>
+  <si>
+    <t>Bits Leftover?</t>
+  </si>
+  <si>
+    <t>CODEC ID?</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>111</t>
   </si>
 </sst>
 </file>
@@ -85,12 +139,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -370,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -381,10 +441,13 @@
     <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="13.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="4"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -394,8 +457,17 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -404,6 +476,165 @@
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3200</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <f>FLOOR($B$2/B3, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="E3" s="1">
+        <f>$B$2-(FLOOR($B$2/B3,1)*B3)</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2400</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" ref="D4:D9" si="0">FLOOR($B$2/B4, 1)</f>
+        <v>4</v>
+      </c>
+      <c r="E4" s="1">
+        <f>$B$2-(FLOOR($B$2/B4,1)*B4)</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" ref="E5:E9" si="1">$B$2-(FLOOR($B$2/B5,1)*B5)</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1400</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="1"/>
+        <v>1200</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1300</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1">
+        <v>700</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F10" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>